<commit_message>
edited resume and programming list
</commit_message>
<xml_diff>
--- a/Programming/Camden_Scholl-Programming_List.xlsx
+++ b/Programming/Camden_Scholl-Programming_List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camde\Documents\professional-documents\Programming\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B7F6BB-299F-4AAC-926B-774B6CF629A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,120 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Camden Scholl Programming List</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>github link</t>
+  </si>
+  <si>
+    <t>heartBeat</t>
+  </si>
+  <si>
+    <t>CABERDLE</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>YouTube Homepage replica</t>
+  </si>
+  <si>
+    <t>Discord Bot</t>
+  </si>
+  <si>
+    <t>JavaScript, node.js</t>
+  </si>
+  <si>
+    <t>https://github.com/c-l-scholl/discord-bot</t>
+  </si>
+  <si>
+    <t>Created a Discord bot that responds to various commands. Followed the instructions on discord.py</t>
+  </si>
+  <si>
+    <t>https://github.com/c-l-scholl/YT-home-page-UI-replica</t>
+  </si>
+  <si>
+    <t>HTML, CSS</t>
+  </si>
+  <si>
+    <t>Practicing a variety of basic HTML and CSS skills. Followed a tutorial by SuperSimpleDev (link in README)</t>
+  </si>
+  <si>
+    <t>Worked with partner to create a more player-friendly version of WORDLE with added difficulty levels and the ability to replay.</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>https://github.com/mac-comp128-s22/128-project-ben-and-camden2</t>
+  </si>
+  <si>
+    <t>Full stack project using Vue.js and Firebase to output Spotify-listed songs based on a user’s heartbeat and mood.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaScript, HTML, CSS, node.js, Vue, Firebase </t>
+  </si>
+  <si>
+    <t>https://github.com/c-l-scholl/stp-vue-fb</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,14 +159,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +480,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{DA6BB4FC-DFBA-4A54-81E5-74B60CEA50CD}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{7DFF2CFE-D8B1-411D-8729-D647BB49BD83}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{80C52AA6-B5F3-48EA-B12A-82A9A8CD4CB8}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{5B335D44-02C4-455A-BF55-C59EE17A2DE0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated resume and programming list
</commit_message>
<xml_diff>
--- a/Programming/Camden_Scholl-Programming_List.xlsx
+++ b/Programming/Camden_Scholl-Programming_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camde\Documents\professional-documents\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B7F6BB-299F-4AAC-926B-774B6CF629A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCC8C12-E5F6-4BD5-B278-3D46231ACD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Camden Scholl Programming List</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>https://github.com/c-l-scholl/stp-vue-fb</t>
+  </si>
+  <si>
+    <t>Packet Sniffer</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>https://github.com/c-l-scholl/python-packet-sniffer</t>
+  </si>
+  <si>
+    <t>Used Python sockets and structs to create a basic packet sniffer. Based on a tutorial by thenewboston</t>
   </si>
 </sst>
 </file>
@@ -481,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,70 +526,85 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{DA6BB4FC-DFBA-4A54-81E5-74B60CEA50CD}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{7DFF2CFE-D8B1-411D-8729-D647BB49BD83}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{80C52AA6-B5F3-48EA-B12A-82A9A8CD4CB8}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{5B335D44-02C4-455A-BF55-C59EE17A2DE0}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{DA6BB4FC-DFBA-4A54-81E5-74B60CEA50CD}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{7DFF2CFE-D8B1-411D-8729-D647BB49BD83}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{80C52AA6-B5F3-48EA-B12A-82A9A8CD4CB8}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{5B335D44-02C4-455A-BF55-C59EE17A2DE0}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{FDA89D95-F2E4-4E49-8C74-2A45823296F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>